<commit_message>
Login page scenarios are added
</commit_message>
<xml_diff>
--- a/src/test/test_data/ipon.xlsx
+++ b/src/test/test_data/ipon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\iponhu\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F749E74C-C0AD-4EBD-B061-849DE49647D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB1B3BA-908A-4169-8B58-5180D59720CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>tc_id</t>
   </si>
@@ -33,24 +33,9 @@
     <t>password</t>
   </si>
   <si>
-    <t>verificationType</t>
-  </si>
-  <si>
-    <t>expectedMessage</t>
-  </si>
-  <si>
-    <t>validEmailPassword</t>
-  </si>
-  <si>
-    <t>PETAR KOCIC</t>
-  </si>
-  <si>
     <t>emptyEmailPasswordMessage2</t>
   </si>
   <si>
-    <t>urlAddressExtension</t>
-  </si>
-  <si>
     <t>Test import data for "Ipon.hu" project</t>
   </si>
   <si>
@@ -115,6 +100,42 @@
   </si>
   <si>
     <t>Kikindski@01</t>
+  </si>
+  <si>
+    <t>languageNumber</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>stjepanovics80@yahoo.com</t>
+  </si>
+  <si>
+    <t>https://iponcomp.com/shop</t>
+  </si>
+  <si>
+    <t>emailYesNo</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>invalidan</t>
+  </si>
+  <si>
+    <t>invalidMessage</t>
+  </si>
+  <si>
+    <t>Invalid credentials.</t>
+  </si>
+  <si>
+    <t>invalid@email</t>
   </si>
 </sst>
 </file>
@@ -239,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -268,6 +289,9 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -583,49 +607,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D05107-472F-4DD1-88F8-DE97CAF36E00}">
-  <dimension ref="A1:AH21"/>
+  <dimension ref="A1:AI21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30" style="1" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24" style="1" customWidth="1"/>
-    <col min="12" max="12" width="20" style="1" customWidth="1"/>
-    <col min="13" max="14" width="17.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="24" style="1" customWidth="1"/>
-    <col min="16" max="17" width="21.5703125" style="1" customWidth="1"/>
-    <col min="18" max="19" width="19.140625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="19.42578125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="19.5703125" style="1" customWidth="1"/>
-    <col min="22" max="23" width="19.140625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="16.5703125" style="1" customWidth="1"/>
-    <col min="25" max="26" width="16.7109375" style="1" customWidth="1"/>
-    <col min="27" max="27" width="17.140625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="16.42578125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="16.140625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="21.140625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="30.85546875" style="1" customWidth="1"/>
-    <col min="32" max="32" width="17" style="1" customWidth="1"/>
-    <col min="33" max="33" width="15.7109375" style="1" customWidth="1"/>
-    <col min="34" max="34" width="14.42578125" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="11" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="21.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="21" style="1" customWidth="1"/>
+    <col min="12" max="12" width="24" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20" style="1" customWidth="1"/>
+    <col min="14" max="15" width="17.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="24" style="1" customWidth="1"/>
+    <col min="17" max="18" width="21.5703125" style="1" customWidth="1"/>
+    <col min="19" max="20" width="19.140625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="19.5703125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="19.140625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="16.5703125" style="1" customWidth="1"/>
+    <col min="26" max="27" width="16.7109375" style="1" customWidth="1"/>
+    <col min="28" max="28" width="17.140625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="16.42578125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="16.140625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="21.140625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="30.85546875" style="1" customWidth="1"/>
+    <col min="33" max="33" width="17" style="1" customWidth="1"/>
+    <col min="34" max="34" width="15.7109375" style="1" customWidth="1"/>
+    <col min="35" max="35" width="14.42578125" style="1" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -660,36 +684,39 @@
       <c r="AF1" s="12"/>
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
-    </row>
-    <row r="2" spans="1:34" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI1" s="12"/>
+    </row>
+    <row r="2" spans="1:35" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
     </row>
-    <row r="3" spans="1:34" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>27</v>
-      </c>
       <c r="H3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
@@ -715,27 +742,30 @@
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="6"/>
-    </row>
-    <row r="4" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI3" s="6"/>
+    </row>
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>4</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
@@ -761,19 +791,32 @@
       <c r="AF4" s="7"/>
       <c r="AG4" s="7"/>
       <c r="AH4" s="7"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI4" s="7"/>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="H5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
@@ -799,19 +842,34 @@
       <c r="AF5" s="7"/>
       <c r="AG5" s="7"/>
       <c r="AH5" s="7"/>
-    </row>
-    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI5" s="7"/>
+    </row>
+    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="H6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
@@ -823,7 +881,7 @@
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
-      <c r="U6" s="8"/>
+      <c r="U6" s="7"/>
       <c r="V6" s="8"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
@@ -834,22 +892,37 @@
       <c r="AC6" s="8"/>
       <c r="AD6" s="8"/>
       <c r="AE6" s="8"/>
-      <c r="AF6" s="7"/>
+      <c r="AF6" s="8"/>
       <c r="AG6" s="7"/>
       <c r="AH6" s="7"/>
-    </row>
-    <row r="7" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI6" s="7"/>
+    </row>
+    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
@@ -861,7 +934,7 @@
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
-      <c r="U7" s="8"/>
+      <c r="U7" s="7"/>
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8"/>
@@ -872,32 +945,45 @@
       <c r="AC7" s="8"/>
       <c r="AD7" s="8"/>
       <c r="AE7" s="8"/>
-      <c r="AF7" s="7"/>
+      <c r="AF7" s="8"/>
       <c r="AG7" s="7"/>
       <c r="AH7" s="7"/>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI7" s="7"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="H8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
-      <c r="N8" s="5"/>
+      <c r="N8" s="7"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
-      <c r="S8" s="7"/>
+      <c r="S8" s="5"/>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
@@ -913,19 +999,32 @@
       <c r="AF8" s="7"/>
       <c r="AG8" s="7"/>
       <c r="AH8" s="7"/>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI8" s="7"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
@@ -937,7 +1036,7 @@
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
-      <c r="U9" s="8"/>
+      <c r="U9" s="7"/>
       <c r="V9" s="8"/>
       <c r="W9" s="8"/>
       <c r="X9" s="8"/>
@@ -948,13 +1047,14 @@
       <c r="AC9" s="8"/>
       <c r="AD9" s="8"/>
       <c r="AE9" s="8"/>
-      <c r="AF9" s="7"/>
+      <c r="AF9" s="8"/>
       <c r="AG9" s="7"/>
       <c r="AH9" s="7"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI9" s="7"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -975,7 +1075,7 @@
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
-      <c r="U10" s="8"/>
+      <c r="U10" s="7"/>
       <c r="V10" s="8"/>
       <c r="W10" s="8"/>
       <c r="X10" s="8"/>
@@ -987,12 +1087,13 @@
       <c r="AD10" s="8"/>
       <c r="AE10" s="8"/>
       <c r="AF10" s="8"/>
-      <c r="AG10" s="7"/>
+      <c r="AG10" s="8"/>
       <c r="AH10" s="7"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI10" s="7"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1003,9 +1104,9 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="5"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="7"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
@@ -1024,13 +1125,14 @@
       <c r="AC11" s="5"/>
       <c r="AD11" s="5"/>
       <c r="AE11" s="5"/>
-      <c r="AF11" s="7"/>
+      <c r="AF11" s="5"/>
       <c r="AG11" s="7"/>
       <c r="AH11" s="7"/>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI11" s="7"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1040,7 +1142,7 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="5"/>
+      <c r="J12" s="7"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -1062,13 +1164,14 @@
       <c r="AC12" s="5"/>
       <c r="AD12" s="5"/>
       <c r="AE12" s="5"/>
-      <c r="AF12" s="7"/>
+      <c r="AF12" s="5"/>
       <c r="AG12" s="7"/>
       <c r="AH12" s="7"/>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI12" s="7"/>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -1078,7 +1181,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="5"/>
+      <c r="J13" s="7"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -1100,13 +1203,14 @@
       <c r="AC13" s="5"/>
       <c r="AD13" s="5"/>
       <c r="AE13" s="5"/>
-      <c r="AF13" s="7"/>
+      <c r="AF13" s="5"/>
       <c r="AG13" s="7"/>
       <c r="AH13" s="7"/>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI13" s="7"/>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -1116,7 +1220,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="5"/>
+      <c r="J14" s="7"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -1138,13 +1242,14 @@
       <c r="AC14" s="5"/>
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
-      <c r="AF14" s="7"/>
+      <c r="AF14" s="5"/>
       <c r="AG14" s="7"/>
       <c r="AH14" s="7"/>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI14" s="7"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1154,7 +1259,7 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="5"/>
+      <c r="J15" s="7"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -1176,13 +1281,14 @@
       <c r="AC15" s="5"/>
       <c r="AD15" s="5"/>
       <c r="AE15" s="5"/>
-      <c r="AF15" s="7"/>
+      <c r="AF15" s="5"/>
       <c r="AG15" s="7"/>
       <c r="AH15" s="7"/>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI15" s="7"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -1192,7 +1298,7 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="5"/>
+      <c r="J16" s="7"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -1203,7 +1309,7 @@
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
-      <c r="U16" s="9"/>
+      <c r="U16" s="5"/>
       <c r="V16" s="9"/>
       <c r="W16" s="9"/>
       <c r="X16" s="9"/>
@@ -1214,13 +1320,14 @@
       <c r="AC16" s="9"/>
       <c r="AD16" s="9"/>
       <c r="AE16" s="9"/>
-      <c r="AF16" s="8"/>
-      <c r="AG16" s="7"/>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="8"/>
       <c r="AH16" s="7"/>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI16" s="7"/>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1230,7 +1337,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="5"/>
+      <c r="J17" s="7"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -1252,23 +1359,24 @@
       <c r="AC17" s="5"/>
       <c r="AD17" s="5"/>
       <c r="AE17" s="5"/>
-      <c r="AF17" s="7"/>
+      <c r="AF17" s="5"/>
       <c r="AG17" s="7"/>
       <c r="AH17" s="7"/>
-    </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI17" s="7"/>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="7"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="5"/>
+      <c r="J18" s="7"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -1292,21 +1400,22 @@
       <c r="AE18" s="5"/>
       <c r="AF18" s="5"/>
       <c r="AG18" s="5"/>
-      <c r="AH18" s="7"/>
-    </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AH18" s="5"/>
+      <c r="AI18" s="7"/>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="7"/>
+      <c r="E19" s="5"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="5"/>
+      <c r="J19" s="7"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
@@ -1330,11 +1439,12 @@
       <c r="AE19" s="5"/>
       <c r="AF19" s="5"/>
       <c r="AG19" s="5"/>
-      <c r="AH19" s="7"/>
-    </row>
-    <row r="20" spans="1:34" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH19" s="5"/>
+      <c r="AI19" s="7"/>
+    </row>
+    <row r="20" spans="1:35" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1369,8 +1479,9 @@
       <c r="AF20" s="7"/>
       <c r="AG20" s="7"/>
       <c r="AH20" s="7"/>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI20" s="7"/>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1380,11 +1491,11 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="5"/>
+      <c r="J21" s="8"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
-      <c r="N21" s="9"/>
+      <c r="N21" s="5"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
       <c r="Q21" s="9"/>
@@ -1402,16 +1513,23 @@
       <c r="AC21" s="9"/>
       <c r="AD21" s="9"/>
       <c r="AE21" s="9"/>
-      <c r="AF21" s="8"/>
-      <c r="AG21" s="7"/>
+      <c r="AF21" s="9"/>
+      <c r="AG21" s="8"/>
       <c r="AH21" s="7"/>
+      <c r="AI21" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:AH1"/>
+    <mergeCell ref="A1:AI1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{38DBEDAC-6A18-4D52-8516-7F6ACE1260D8}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{8CB34109-BDAD-4F13-B287-562F9318C628}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{F528F4DF-3477-4E50-98F5-E358FC6EF63E}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{C48B9FC7-84F8-4564-8301-99766A139742}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Footer feature and page are added. Gitignore file has changed
</commit_message>
<xml_diff>
--- a/src/test/test_data/ipon.xlsx
+++ b/src/test/test_data/ipon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\iponhu\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB1B3BA-908A-4169-8B58-5180D59720CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78775E2A-F0B0-4251-A136-C88B3B18BA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="4" r:id="rId1"/>
@@ -114,9 +114,6 @@
     <t>stjepanovics80@yahoo.com</t>
   </si>
   <si>
-    <t>https://iponcomp.com/shop</t>
-  </si>
-  <si>
     <t>emailYesNo</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>invalid@email</t>
+  </si>
+  <si>
+    <t>https://ipon.hu</t>
   </si>
 </sst>
 </file>
@@ -284,14 +284,14 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,7 +610,7 @@
   <dimension ref="A1:AI21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,43 +648,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="13"/>
     </row>
     <row r="2" spans="1:35" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -703,10 +703,10 @@
         <v>27</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>2</v>
@@ -756,14 +756,14 @@
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>26</v>
       </c>
       <c r="J4" s="7"/>
@@ -807,14 +807,14 @@
         <v>28</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>26</v>
       </c>
       <c r="J5" s="7"/>
@@ -849,7 +849,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>24</v>
@@ -858,16 +858,16 @@
         <v>28</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>26</v>
       </c>
       <c r="J6" s="7"/>
@@ -908,19 +908,19 @@
         <v>24</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="11" t="s">
         <v>26</v>
       </c>
       <c r="J7" s="7"/>
@@ -959,19 +959,19 @@
         <v>24</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="11" t="s">
         <v>26</v>
       </c>
       <c r="J8" s="7"/>
@@ -1013,16 +1013,16 @@
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>26</v>
       </c>
       <c r="J9" s="7"/>
@@ -1528,8 +1528,10 @@
     <hyperlink ref="D5" r:id="rId2" xr:uid="{8CB34109-BDAD-4F13-B287-562F9318C628}"/>
     <hyperlink ref="C6" r:id="rId3" xr:uid="{F528F4DF-3477-4E50-98F5-E358FC6EF63E}"/>
     <hyperlink ref="D6" r:id="rId4" xr:uid="{C48B9FC7-84F8-4564-8301-99766A139742}"/>
+    <hyperlink ref="H4" r:id="rId5" xr:uid="{FF2CD2B1-E565-472B-91C8-0A0D6E475D22}"/>
+    <hyperlink ref="H5:H9" r:id="rId6" display="https://ipon.hu" xr:uid="{A350EFC6-9B6A-4372-8867-11A394D16443}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
registration scenarios are added
</commit_message>
<xml_diff>
--- a/src/test/test_data/ipon.xlsx
+++ b/src/test/test_data/ipon.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\iponhu\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78775E2A-F0B0-4251-A136-C88B3B18BA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55ED2BE-41DB-45EC-9994-684F0B737647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
-    <sheet name="general" sheetId="4" r:id="rId1"/>
+    <sheet name="login" sheetId="4" r:id="rId1"/>
+    <sheet name="registration" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="59">
   <si>
     <t>tc_id</t>
   </si>
@@ -135,7 +137,73 @@
     <t>invalid@email</t>
   </si>
   <si>
-    <t>https://ipon.hu</t>
+    <t>https://iponcomp.com/shop</t>
+  </si>
+  <si>
+    <t>logIn</t>
+  </si>
+  <si>
+    <t>logOut</t>
+  </si>
+  <si>
+    <t>Log in</t>
+  </si>
+  <si>
+    <t>My profile</t>
+  </si>
+  <si>
+    <t>url2</t>
+  </si>
+  <si>
+    <t>https://iponcomp.com/lost-password</t>
+  </si>
+  <si>
+    <t>https://iponcomp.com/registration</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>randomTypeYesNo</t>
+  </si>
+  <si>
+    <t>emailRegistration</t>
+  </si>
+  <si>
+    <t>passwordRegistration</t>
+  </si>
+  <si>
+    <t>userNameRegistration</t>
+  </si>
+  <si>
+    <t>Nikolic</t>
+  </si>
+  <si>
+    <t>Dragan</t>
+  </si>
+  <si>
+    <t>url3</t>
+  </si>
+  <si>
+    <t>https://iponcomp.com/login</t>
+  </si>
+  <si>
+    <t>errorMessageEmpty</t>
+  </si>
+  <si>
+    <t>This value should not be blank.</t>
+  </si>
+  <si>
+    <t>This value is not a valid email address.</t>
+  </si>
+  <si>
+    <t>errorMesssageEmailNotValid</t>
+  </si>
+  <si>
+    <t>empty</t>
   </si>
 </sst>
 </file>
@@ -299,6 +367,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -607,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D05107-472F-4DD1-88F8-DE97CAF36E00}">
-  <dimension ref="A1:AI21"/>
+  <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,36 +691,38 @@
     <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="21.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="29.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="21" style="1" customWidth="1"/>
-    <col min="12" max="12" width="24" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20" style="1" customWidth="1"/>
-    <col min="14" max="15" width="17.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="24" style="1" customWidth="1"/>
-    <col min="17" max="18" width="21.5703125" style="1" customWidth="1"/>
-    <col min="19" max="20" width="19.140625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="19.140625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="16.5703125" style="1" customWidth="1"/>
-    <col min="26" max="27" width="16.7109375" style="1" customWidth="1"/>
-    <col min="28" max="28" width="17.140625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="16.42578125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="16.140625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="21.140625" style="1" customWidth="1"/>
-    <col min="32" max="32" width="30.85546875" style="1" customWidth="1"/>
-    <col min="33" max="33" width="17" style="1" customWidth="1"/>
-    <col min="34" max="34" width="15.7109375" style="1" customWidth="1"/>
-    <col min="35" max="35" width="14.42578125" style="1" customWidth="1"/>
-    <col min="36" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="26.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21" style="1" customWidth="1"/>
+    <col min="13" max="13" width="24" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20" style="1" customWidth="1"/>
+    <col min="15" max="16" width="17.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="24" style="1" customWidth="1"/>
+    <col min="18" max="19" width="21.5703125" style="1" customWidth="1"/>
+    <col min="20" max="21" width="19.140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="19.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" style="1" customWidth="1"/>
+    <col min="24" max="25" width="19.140625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="16.5703125" style="1" customWidth="1"/>
+    <col min="27" max="28" width="16.7109375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="17.140625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="16.42578125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="16.140625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="21.140625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="30.85546875" style="1" customWidth="1"/>
+    <col min="34" max="34" width="17" style="1" customWidth="1"/>
+    <col min="35" max="35" width="15.7109375" style="1" customWidth="1"/>
+    <col min="36" max="36" width="14.42578125" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -685,11 +760,12 @@
       <c r="AG1" s="13"/>
       <c r="AH1" s="13"/>
       <c r="AI1" s="13"/>
-    </row>
-    <row r="2" spans="1:35" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ1" s="13"/>
+    </row>
+    <row r="2" spans="1:36" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
     </row>
-    <row r="3" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -715,11 +791,17 @@
         <v>22</v>
       </c>
       <c r="I3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+      <c r="K3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
@@ -743,8 +825,9 @@
       <c r="AG3" s="6"/>
       <c r="AH3" s="6"/>
       <c r="AI3" s="6"/>
-    </row>
-    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ3" s="6"/>
+    </row>
+    <row r="4" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -763,12 +846,18 @@
       <c r="H4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
+      <c r="K4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -792,8 +881,9 @@
       <c r="AG4" s="7"/>
       <c r="AH4" s="7"/>
       <c r="AI4" s="7"/>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ4" s="7"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -814,12 +904,16 @@
       <c r="H5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="7"/>
+      <c r="J5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
+      <c r="K5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
@@ -843,8 +937,9 @@
       <c r="AG5" s="7"/>
       <c r="AH5" s="7"/>
       <c r="AI5" s="7"/>
-    </row>
-    <row r="6" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ5" s="7"/>
+    </row>
+    <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -867,10 +962,10 @@
       <c r="H6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="7"/>
+      <c r="J6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -882,7 +977,7 @@
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
-      <c r="V6" s="8"/>
+      <c r="V6" s="7"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
@@ -893,11 +988,12 @@
       <c r="AD6" s="8"/>
       <c r="AE6" s="8"/>
       <c r="AF6" s="8"/>
-      <c r="AG6" s="7"/>
+      <c r="AG6" s="8"/>
       <c r="AH6" s="7"/>
       <c r="AI6" s="7"/>
-    </row>
-    <row r="7" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ6" s="7"/>
+    </row>
+    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -920,10 +1016,10 @@
       <c r="H7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="7"/>
+      <c r="J7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
@@ -935,7 +1031,7 @@
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
-      <c r="V7" s="8"/>
+      <c r="V7" s="7"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8"/>
       <c r="Y7" s="8"/>
@@ -946,11 +1042,12 @@
       <c r="AD7" s="8"/>
       <c r="AE7" s="8"/>
       <c r="AF7" s="8"/>
-      <c r="AG7" s="7"/>
+      <c r="AG7" s="8"/>
       <c r="AH7" s="7"/>
       <c r="AI7" s="7"/>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ7" s="7"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -971,20 +1068,20 @@
       <c r="H8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="7"/>
+      <c r="J8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
-      <c r="O8" s="5"/>
+      <c r="O8" s="7"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
-      <c r="T8" s="7"/>
+      <c r="T8" s="5"/>
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
@@ -1000,8 +1097,9 @@
       <c r="AG8" s="7"/>
       <c r="AH8" s="7"/>
       <c r="AI8" s="7"/>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ8" s="7"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -1022,10 +1120,10 @@
       <c r="H9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="7"/>
+      <c r="J9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
@@ -1037,7 +1135,7 @@
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
-      <c r="V9" s="8"/>
+      <c r="V9" s="7"/>
       <c r="W9" s="8"/>
       <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
@@ -1048,11 +1146,12 @@
       <c r="AD9" s="8"/>
       <c r="AE9" s="8"/>
       <c r="AF9" s="8"/>
-      <c r="AG9" s="7"/>
+      <c r="AG9" s="8"/>
       <c r="AH9" s="7"/>
       <c r="AI9" s="7"/>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ9" s="7"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -1076,7 +1175,7 @@
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
-      <c r="V10" s="8"/>
+      <c r="V10" s="7"/>
       <c r="W10" s="8"/>
       <c r="X10" s="8"/>
       <c r="Y10" s="8"/>
@@ -1088,10 +1187,11 @@
       <c r="AE10" s="8"/>
       <c r="AF10" s="8"/>
       <c r="AG10" s="8"/>
-      <c r="AH10" s="7"/>
+      <c r="AH10" s="8"/>
       <c r="AI10" s="7"/>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ10" s="7"/>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1105,9 +1205,9 @@
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="5"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="7"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
@@ -1126,11 +1226,12 @@
       <c r="AD11" s="5"/>
       <c r="AE11" s="5"/>
       <c r="AF11" s="5"/>
-      <c r="AG11" s="7"/>
+      <c r="AG11" s="5"/>
       <c r="AH11" s="7"/>
       <c r="AI11" s="7"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ11" s="7"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -1143,7 +1244,7 @@
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="5"/>
+      <c r="K12" s="7"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
@@ -1165,11 +1266,12 @@
       <c r="AD12" s="5"/>
       <c r="AE12" s="5"/>
       <c r="AF12" s="5"/>
-      <c r="AG12" s="7"/>
+      <c r="AG12" s="5"/>
       <c r="AH12" s="7"/>
       <c r="AI12" s="7"/>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ12" s="7"/>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -1182,7 +1284,7 @@
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="5"/>
+      <c r="K13" s="7"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -1204,11 +1306,12 @@
       <c r="AD13" s="5"/>
       <c r="AE13" s="5"/>
       <c r="AF13" s="5"/>
-      <c r="AG13" s="7"/>
+      <c r="AG13" s="5"/>
       <c r="AH13" s="7"/>
       <c r="AI13" s="7"/>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ13" s="7"/>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -1221,7 +1324,7 @@
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="5"/>
+      <c r="K14" s="7"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
@@ -1243,11 +1346,12 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
       <c r="AF14" s="5"/>
-      <c r="AG14" s="7"/>
+      <c r="AG14" s="5"/>
       <c r="AH14" s="7"/>
       <c r="AI14" s="7"/>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ14" s="7"/>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -1260,7 +1364,7 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="5"/>
+      <c r="K15" s="7"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
@@ -1282,11 +1386,12 @@
       <c r="AD15" s="5"/>
       <c r="AE15" s="5"/>
       <c r="AF15" s="5"/>
-      <c r="AG15" s="7"/>
+      <c r="AG15" s="5"/>
       <c r="AH15" s="7"/>
       <c r="AI15" s="7"/>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ15" s="7"/>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -1299,7 +1404,7 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="5"/>
+      <c r="K16" s="7"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
@@ -1310,7 +1415,7 @@
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
       <c r="U16" s="5"/>
-      <c r="V16" s="9"/>
+      <c r="V16" s="5"/>
       <c r="W16" s="9"/>
       <c r="X16" s="9"/>
       <c r="Y16" s="9"/>
@@ -1321,11 +1426,12 @@
       <c r="AD16" s="9"/>
       <c r="AE16" s="9"/>
       <c r="AF16" s="9"/>
-      <c r="AG16" s="8"/>
-      <c r="AH16" s="7"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="8"/>
       <c r="AI16" s="7"/>
-    </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ16" s="7"/>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -1338,7 +1444,7 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
-      <c r="K17" s="5"/>
+      <c r="K17" s="7"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
@@ -1360,11 +1466,12 @@
       <c r="AD17" s="5"/>
       <c r="AE17" s="5"/>
       <c r="AF17" s="5"/>
-      <c r="AG17" s="7"/>
+      <c r="AG17" s="5"/>
       <c r="AH17" s="7"/>
       <c r="AI17" s="7"/>
-    </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ17" s="7"/>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
@@ -1377,7 +1484,7 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
-      <c r="K18" s="5"/>
+      <c r="K18" s="7"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
@@ -1401,9 +1508,10 @@
       <c r="AF18" s="5"/>
       <c r="AG18" s="5"/>
       <c r="AH18" s="5"/>
-      <c r="AI18" s="7"/>
-    </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AI18" s="5"/>
+      <c r="AJ18" s="7"/>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
@@ -1416,7 +1524,7 @@
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
-      <c r="K19" s="5"/>
+      <c r="K19" s="7"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
@@ -1440,9 +1548,10 @@
       <c r="AF19" s="5"/>
       <c r="AG19" s="5"/>
       <c r="AH19" s="5"/>
-      <c r="AI19" s="7"/>
-    </row>
-    <row r="20" spans="1:35" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI19" s="5"/>
+      <c r="AJ19" s="7"/>
+    </row>
+    <row r="20" spans="1:36" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -1480,8 +1589,9 @@
       <c r="AG20" s="7"/>
       <c r="AH20" s="7"/>
       <c r="AI20" s="7"/>
-    </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ20" s="7"/>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1492,11 +1602,11 @@
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
-      <c r="K21" s="5"/>
+      <c r="K21" s="8"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
-      <c r="O21" s="9"/>
+      <c r="O21" s="5"/>
       <c r="P21" s="9"/>
       <c r="Q21" s="9"/>
       <c r="R21" s="9"/>
@@ -1514,24 +1624,1142 @@
       <c r="AD21" s="9"/>
       <c r="AE21" s="9"/>
       <c r="AF21" s="9"/>
-      <c r="AG21" s="8"/>
-      <c r="AH21" s="7"/>
+      <c r="AG21" s="9"/>
+      <c r="AH21" s="8"/>
       <c r="AI21" s="7"/>
+      <c r="AJ21" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:AI1"/>
+    <mergeCell ref="A1:AJ1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" xr:uid="{38DBEDAC-6A18-4D52-8516-7F6ACE1260D8}"/>
-    <hyperlink ref="D5" r:id="rId2" xr:uid="{8CB34109-BDAD-4F13-B287-562F9318C628}"/>
-    <hyperlink ref="C6" r:id="rId3" xr:uid="{F528F4DF-3477-4E50-98F5-E358FC6EF63E}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{C48B9FC7-84F8-4564-8301-99766A139742}"/>
-    <hyperlink ref="H4" r:id="rId5" xr:uid="{FF2CD2B1-E565-472B-91C8-0A0D6E475D22}"/>
-    <hyperlink ref="H5:H9" r:id="rId6" display="https://ipon.hu" xr:uid="{A350EFC6-9B6A-4372-8867-11A394D16443}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{F528F4DF-3477-4E50-98F5-E358FC6EF63E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B244FFE7-0967-47E4-BD24-686C74F1C03E}">
+  <dimension ref="A1:AP21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="1" customWidth="1"/>
+    <col min="7" max="8" width="15.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22" style="1" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20" style="1" customWidth="1"/>
+    <col min="14" max="14" width="26.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="19.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="8" style="1" customWidth="1"/>
+    <col min="19" max="19" width="23" style="1" customWidth="1"/>
+    <col min="20" max="20" width="28.28515625" style="1" customWidth="1"/>
+    <col min="21" max="22" width="17.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="24" style="1" customWidth="1"/>
+    <col min="24" max="25" width="21.5703125" style="1" customWidth="1"/>
+    <col min="26" max="27" width="19.140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="19.42578125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" style="1" customWidth="1"/>
+    <col min="30" max="31" width="19.140625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="16.5703125" style="1" customWidth="1"/>
+    <col min="33" max="34" width="16.7109375" style="1" customWidth="1"/>
+    <col min="35" max="35" width="17.140625" style="1" customWidth="1"/>
+    <col min="36" max="36" width="16.42578125" style="1" customWidth="1"/>
+    <col min="37" max="37" width="16.140625" style="1" customWidth="1"/>
+    <col min="38" max="38" width="21.140625" style="1" customWidth="1"/>
+    <col min="39" max="39" width="30.85546875" style="1" customWidth="1"/>
+    <col min="40" max="40" width="17" style="1" customWidth="1"/>
+    <col min="41" max="41" width="15.7109375" style="1" customWidth="1"/>
+    <col min="42" max="42" width="14.42578125" style="1" customWidth="1"/>
+    <col min="43" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="13"/>
+      <c r="AJ1" s="13"/>
+      <c r="AK1" s="13"/>
+      <c r="AL1" s="13"/>
+      <c r="AM1" s="13"/>
+      <c r="AN1" s="13"/>
+      <c r="AO1" s="13"/>
+      <c r="AP1" s="13"/>
+    </row>
+    <row r="2" spans="1:42" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+    </row>
+    <row r="3" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+      <c r="AK3" s="6"/>
+      <c r="AL3" s="6"/>
+      <c r="AM3" s="6"/>
+      <c r="AN3" s="6"/>
+      <c r="AO3" s="6"/>
+      <c r="AP3" s="6"/>
+    </row>
+    <row r="4" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" s="7"/>
+      <c r="P4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
+      <c r="AG4" s="7"/>
+      <c r="AH4" s="7"/>
+      <c r="AI4" s="7"/>
+      <c r="AJ4" s="7"/>
+      <c r="AK4" s="7"/>
+      <c r="AL4" s="7"/>
+      <c r="AM4" s="7"/>
+      <c r="AN4" s="7"/>
+      <c r="AO4" s="7"/>
+      <c r="AP4" s="7"/>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7"/>
+      <c r="AJ5" s="7"/>
+      <c r="AK5" s="7"/>
+      <c r="AL5" s="7"/>
+      <c r="AM5" s="7"/>
+      <c r="AN5" s="7"/>
+      <c r="AO5" s="7"/>
+      <c r="AP5" s="7"/>
+    </row>
+    <row r="6" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="8"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
+      <c r="AJ6" s="8"/>
+      <c r="AK6" s="8"/>
+      <c r="AL6" s="8"/>
+      <c r="AM6" s="8"/>
+      <c r="AN6" s="7"/>
+      <c r="AO6" s="7"/>
+      <c r="AP6" s="7"/>
+    </row>
+    <row r="7" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="8"/>
+      <c r="AF7" s="8"/>
+      <c r="AG7" s="8"/>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="8"/>
+      <c r="AJ7" s="8"/>
+      <c r="AK7" s="8"/>
+      <c r="AL7" s="8"/>
+      <c r="AM7" s="8"/>
+      <c r="AN7" s="7"/>
+      <c r="AO7" s="7"/>
+      <c r="AP7" s="7"/>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="7"/>
+      <c r="AL8" s="7"/>
+      <c r="AM8" s="7"/>
+      <c r="AN8" s="7"/>
+      <c r="AO8" s="7"/>
+      <c r="AP8" s="7"/>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="8"/>
+      <c r="AG9" s="8"/>
+      <c r="AH9" s="8"/>
+      <c r="AI9" s="8"/>
+      <c r="AJ9" s="8"/>
+      <c r="AK9" s="8"/>
+      <c r="AL9" s="8"/>
+      <c r="AM9" s="8"/>
+      <c r="AN9" s="7"/>
+      <c r="AO9" s="7"/>
+      <c r="AP9" s="7"/>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8"/>
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="8"/>
+      <c r="AG10" s="8"/>
+      <c r="AH10" s="8"/>
+      <c r="AI10" s="8"/>
+      <c r="AJ10" s="8"/>
+      <c r="AK10" s="8"/>
+      <c r="AL10" s="8"/>
+      <c r="AM10" s="8"/>
+      <c r="AN10" s="8"/>
+      <c r="AO10" s="7"/>
+      <c r="AP10" s="7"/>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5"/>
+      <c r="AE11" s="5"/>
+      <c r="AF11" s="5"/>
+      <c r="AG11" s="5"/>
+      <c r="AH11" s="5"/>
+      <c r="AI11" s="5"/>
+      <c r="AJ11" s="5"/>
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="5"/>
+      <c r="AM11" s="5"/>
+      <c r="AN11" s="7"/>
+      <c r="AO11" s="7"/>
+      <c r="AP11" s="7"/>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="5"/>
+      <c r="AE12" s="5"/>
+      <c r="AF12" s="5"/>
+      <c r="AG12" s="5"/>
+      <c r="AH12" s="5"/>
+      <c r="AI12" s="5"/>
+      <c r="AJ12" s="5"/>
+      <c r="AK12" s="5"/>
+      <c r="AL12" s="5"/>
+      <c r="AM12" s="5"/>
+      <c r="AN12" s="7"/>
+      <c r="AO12" s="7"/>
+      <c r="AP12" s="7"/>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="5"/>
+      <c r="AE13" s="5"/>
+      <c r="AF13" s="5"/>
+      <c r="AG13" s="5"/>
+      <c r="AH13" s="5"/>
+      <c r="AI13" s="5"/>
+      <c r="AJ13" s="5"/>
+      <c r="AK13" s="5"/>
+      <c r="AL13" s="5"/>
+      <c r="AM13" s="5"/>
+      <c r="AN13" s="7"/>
+      <c r="AO13" s="7"/>
+      <c r="AP13" s="7"/>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="5"/>
+      <c r="AI14" s="5"/>
+      <c r="AJ14" s="5"/>
+      <c r="AK14" s="5"/>
+      <c r="AL14" s="5"/>
+      <c r="AM14" s="5"/>
+      <c r="AN14" s="7"/>
+      <c r="AO14" s="7"/>
+      <c r="AP14" s="7"/>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="5"/>
+      <c r="AE15" s="5"/>
+      <c r="AF15" s="5"/>
+      <c r="AG15" s="5"/>
+      <c r="AH15" s="5"/>
+      <c r="AI15" s="5"/>
+      <c r="AJ15" s="5"/>
+      <c r="AK15" s="5"/>
+      <c r="AL15" s="5"/>
+      <c r="AM15" s="5"/>
+      <c r="AN15" s="7"/>
+      <c r="AO15" s="7"/>
+      <c r="AP15" s="7"/>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="9"/>
+      <c r="AI16" s="9"/>
+      <c r="AJ16" s="9"/>
+      <c r="AK16" s="9"/>
+      <c r="AL16" s="9"/>
+      <c r="AM16" s="9"/>
+      <c r="AN16" s="8"/>
+      <c r="AO16" s="7"/>
+      <c r="AP16" s="7"/>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="5"/>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="5"/>
+      <c r="AG17" s="5"/>
+      <c r="AH17" s="5"/>
+      <c r="AI17" s="5"/>
+      <c r="AJ17" s="5"/>
+      <c r="AK17" s="5"/>
+      <c r="AL17" s="5"/>
+      <c r="AM17" s="5"/>
+      <c r="AN17" s="7"/>
+      <c r="AO17" s="7"/>
+      <c r="AP17" s="7"/>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="5"/>
+      <c r="AF18" s="5"/>
+      <c r="AG18" s="5"/>
+      <c r="AH18" s="5"/>
+      <c r="AI18" s="5"/>
+      <c r="AJ18" s="5"/>
+      <c r="AK18" s="5"/>
+      <c r="AL18" s="5"/>
+      <c r="AM18" s="5"/>
+      <c r="AN18" s="5"/>
+      <c r="AO18" s="5"/>
+      <c r="AP18" s="7"/>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
+      <c r="AF19" s="5"/>
+      <c r="AG19" s="5"/>
+      <c r="AH19" s="5"/>
+      <c r="AI19" s="5"/>
+      <c r="AJ19" s="5"/>
+      <c r="AK19" s="5"/>
+      <c r="AL19" s="5"/>
+      <c r="AM19" s="5"/>
+      <c r="AN19" s="5"/>
+      <c r="AO19" s="5"/>
+      <c r="AP19" s="7"/>
+    </row>
+    <row r="20" spans="1:42" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="7"/>
+      <c r="AF20" s="7"/>
+      <c r="AG20" s="7"/>
+      <c r="AH20" s="7"/>
+      <c r="AI20" s="7"/>
+      <c r="AJ20" s="7"/>
+      <c r="AK20" s="7"/>
+      <c r="AL20" s="7"/>
+      <c r="AM20" s="7"/>
+      <c r="AN20" s="7"/>
+      <c r="AO20" s="7"/>
+      <c r="AP20" s="7"/>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="9"/>
+      <c r="AG21" s="9"/>
+      <c r="AH21" s="9"/>
+      <c r="AI21" s="9"/>
+      <c r="AJ21" s="9"/>
+      <c r="AK21" s="9"/>
+      <c r="AL21" s="9"/>
+      <c r="AM21" s="9"/>
+      <c r="AN21" s="8"/>
+      <c r="AO21" s="7"/>
+      <c r="AP21" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AP1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{8F7995FC-AE38-475B-9CCF-F03437F345FA}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{2C1026B0-81E6-4D41-8C97-55B34C3C5182}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Apply filter is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/ipon.xlsx
+++ b/src/test/test_data/ipon.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\iponhu\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55ED2BE-41DB-45EC-9994-684F0B737647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB044E80-DD14-4531-AB66-AC33AFDF98D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="4" r:id="rId1"/>
     <sheet name="registration" sheetId="5" r:id="rId2"/>
+    <sheet name="notebook" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="110">
   <si>
     <t>tc_id</t>
   </si>
@@ -204,6 +204,159 @@
   </si>
   <si>
     <t>empty</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>This value is too short. It should have 6 characters or more.</t>
+  </si>
+  <si>
+    <t>kikon</t>
+  </si>
+  <si>
+    <t>This value is too long. It should have 30 characters or less.</t>
+  </si>
+  <si>
+    <t>kikonkikonkikonkikonkikonkikon1</t>
+  </si>
+  <si>
+    <t>ORDERS</t>
+  </si>
+  <si>
+    <t>FAVOURITES</t>
+  </si>
+  <si>
+    <t>MONITORED ITEMS</t>
+  </si>
+  <si>
+    <t>PARTNER PROGRAM</t>
+  </si>
+  <si>
+    <t>PERSONAL INFORMATION</t>
+  </si>
+  <si>
+    <t>SETTINGS</t>
+  </si>
+  <si>
+    <t>myProfileItem1</t>
+  </si>
+  <si>
+    <t>myProfileItem2</t>
+  </si>
+  <si>
+    <t>myProfileItem3</t>
+  </si>
+  <si>
+    <t>myProfileItem4</t>
+  </si>
+  <si>
+    <t>myProfileItem5</t>
+  </si>
+  <si>
+    <t>myProfileItem6</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>subCategory</t>
+  </si>
+  <si>
+    <t>Headset</t>
+  </si>
+  <si>
+    <t>PC accessories</t>
+  </si>
+  <si>
+    <t>notebook</t>
+  </si>
+  <si>
+    <t>Notebook, PC, eBook</t>
+  </si>
+  <si>
+    <t>Notebook</t>
+  </si>
+  <si>
+    <t>typeFilterNotebook</t>
+  </si>
+  <si>
+    <t>minPrice</t>
+  </si>
+  <si>
+    <t>maxPrice</t>
+  </si>
+  <si>
+    <t>pickup</t>
+  </si>
+  <si>
+    <t>2 days</t>
+  </si>
+  <si>
+    <t>warrantyMax</t>
+  </si>
+  <si>
+    <t>warrantyMin</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Notebook accessories</t>
+  </si>
+  <si>
+    <t>APPLE</t>
+  </si>
+  <si>
+    <t>11000'</t>
+  </si>
+  <si>
+    <t>80000'</t>
+  </si>
+  <si>
+    <t>DELL</t>
+  </si>
+  <si>
+    <t>ANKER</t>
+  </si>
+  <si>
+    <t>110000'</t>
+  </si>
+  <si>
+    <t>132000'</t>
+  </si>
+  <si>
+    <t>1 days</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>noFilteredAction</t>
+  </si>
+  <si>
+    <t>Sadly, there is no result we can show you!</t>
+  </si>
+  <si>
+    <t>LENOVO</t>
+  </si>
+  <si>
+    <t>150000</t>
+  </si>
+  <si>
+    <t>250000</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>24</t>
   </si>
 </sst>
 </file>
@@ -261,7 +414,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +430,12 @@
           <color theme="5" tint="0.40000610370189521"/>
         </stop>
       </gradientFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -328,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -355,10 +514,19 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -683,7 +851,7 @@
   <dimension ref="A1:AJ21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,15 +865,17 @@
     <col min="7" max="7" width="29.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="1" customWidth="1"/>
     <col min="9" max="9" width="26.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="21" style="1" customWidth="1"/>
-    <col min="13" max="13" width="24" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="20" style="1" customWidth="1"/>
     <col min="15" max="16" width="17.42578125" style="1" customWidth="1"/>
     <col min="17" max="17" width="24" style="1" customWidth="1"/>
-    <col min="18" max="19" width="21.5703125" style="1" customWidth="1"/>
-    <col min="20" max="21" width="19.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" style="1" customWidth="1"/>
     <col min="22" max="22" width="19.42578125" style="1" customWidth="1"/>
     <col min="23" max="23" width="19.5703125" style="1" customWidth="1"/>
     <col min="24" max="25" width="19.140625" style="1" customWidth="1"/>
@@ -723,44 +893,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="14"/>
     </row>
     <row r="2" spans="1:36" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -802,14 +972,30 @@
       <c r="L3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
+      <c r="M3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
@@ -858,14 +1044,30 @@
       <c r="L4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
+      <c r="M4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="U4" s="7"/>
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
@@ -914,7 +1116,7 @@
       <c r="L5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="M5" s="7"/>
+      <c r="M5" s="5"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
@@ -968,7 +1170,7 @@
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="M6" s="5"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -1022,7 +1224,7 @@
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
+      <c r="M7" s="5"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
@@ -1074,7 +1276,7 @@
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="M8" s="5"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="5"/>
@@ -1126,7 +1328,7 @@
       </c>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
+      <c r="M9" s="5"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
@@ -1647,8 +1849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B244FFE7-0967-47E4-BD24-686C74F1C03E}">
   <dimension ref="A1:AP21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,50 +1895,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="14"/>
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="14"/>
     </row>
     <row r="2" spans="1:42" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
@@ -2058,7 +2260,9 @@
       </c>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
+      <c r="S7" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="T7" s="7" t="s">
         <v>56</v>
       </c>
@@ -2085,7 +2289,7 @@
       <c r="AO7" s="7"/>
       <c r="AP7" s="7"/>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -2105,7 +2309,9 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="J8" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7" t="s">
@@ -2118,8 +2324,12 @@
       </c>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
+      <c r="S8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="U8" s="7"/>
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
@@ -2143,7 +2353,7 @@
       <c r="AO8" s="7"/>
       <c r="AP8" s="7"/>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -2153,7 +2363,9 @@
       <c r="C9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="E9" s="7" t="s">
         <v>31</v>
       </c>
@@ -2164,7 +2376,9 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+      <c r="K9" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="L9" s="7"/>
       <c r="M9" s="7" t="s">
         <v>36</v>
@@ -2176,8 +2390,12 @@
       </c>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
+      <c r="S9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="U9" s="7"/>
       <c r="V9" s="7"/>
       <c r="W9" s="7"/>
@@ -2201,29 +2419,47 @@
       <c r="AO9" s="7"/>
       <c r="AP9" s="7"/>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="B10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
+      <c r="K10" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="M10" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
+      <c r="P10" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
+      <c r="T10" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="U10" s="7"/>
       <c r="V10" s="7"/>
       <c r="W10" s="7"/>
@@ -2762,4 +2998,934 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BD2F75-093A-4CCC-AFDF-54FE23EAD35D}">
+  <dimension ref="A1:AF21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="19.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" style="1" customWidth="1"/>
+    <col min="20" max="21" width="19.140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="16.5703125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="16.7109375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="17.140625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="16.140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="21.140625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="30.85546875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="17" style="1" customWidth="1"/>
+    <col min="31" max="31" width="15.7109375" style="1" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+    </row>
+    <row r="2" spans="1:32" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+    </row>
+    <row r="3" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="12"/>
+      <c r="AA3" s="12"/>
+      <c r="AB3" s="12"/>
+      <c r="AC3" s="12"/>
+      <c r="AD3" s="12"/>
+      <c r="AE3" s="12"/>
+      <c r="AF3" s="12"/>
+    </row>
+    <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
+    </row>
+    <row r="5" spans="1:32" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+    </row>
+    <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+    </row>
+    <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="7"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="7"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="8"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="5"/>
+      <c r="AF18" s="7"/>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
+      <c r="AF19" s="7"/>
+    </row>
+    <row r="20" spans="1:32" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="7"/>
+      <c r="AF20" s="7"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="8"/>
+      <c r="AE21" s="7"/>
+      <c r="AF21" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AF1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{36A369D6-E91B-49AE-8B24-4F98FC641AA4}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{0703A915-9653-412D-B56E-A64DD871DA0F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Checkout page is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/ipon.xlsx
+++ b/src/test/test_data/ipon.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\iponhu\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB044E80-DD14-4531-AB66-AC33AFDF98D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23663BE-FA2C-4087-B615-A776D132DF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="4" r:id="rId1"/>
     <sheet name="registration" sheetId="5" r:id="rId2"/>
     <sheet name="notebook" sheetId="6" r:id="rId3"/>
+    <sheet name="checkout" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="121">
   <si>
     <t>tc_id</t>
   </si>
@@ -357,6 +358,39 @@
   </si>
   <si>
     <t>24</t>
+  </si>
+  <si>
+    <t>emptyBasket</t>
+  </si>
+  <si>
+    <t>YOUR CART IS EMPTY!</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>attributeType</t>
+  </si>
+  <si>
+    <t>background-color</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>rgba(239, 68, 68, 1)</t>
+  </si>
+  <si>
+    <t>zipcodeMessage</t>
+  </si>
+  <si>
+    <t>cityMessage</t>
+  </si>
+  <si>
+    <t>streetMessage</t>
   </si>
 </sst>
 </file>
@@ -414,7 +448,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,6 +469,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -487,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -528,6 +568,15 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3004,8 +3053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BD2F75-093A-4CCC-AFDF-54FE23EAD35D}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3027,7 +3076,7 @@
     <col min="15" max="15" width="11.5703125" style="1" customWidth="1"/>
     <col min="16" max="16" width="14.28515625" style="1" customWidth="1"/>
     <col min="17" max="17" width="17.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="19.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" style="1" customWidth="1"/>
     <col min="19" max="19" width="19.5703125" style="1" customWidth="1"/>
     <col min="20" max="21" width="19.140625" style="1" customWidth="1"/>
     <col min="22" max="22" width="16.5703125" style="1" customWidth="1"/>
@@ -3134,10 +3183,18 @@
       <c r="Q3" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
+      <c r="R3" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="S3" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="U3" s="12" t="s">
+        <v>116</v>
+      </c>
       <c r="V3" s="12"/>
       <c r="W3" s="12"/>
       <c r="X3" s="12"/>
@@ -3200,8 +3257,12 @@
         <v>91</v>
       </c>
       <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
+      <c r="R4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>113</v>
+      </c>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
       <c r="V4" s="7"/>
@@ -3266,8 +3327,12 @@
       <c r="Q5" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
+      <c r="R5" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>113</v>
+      </c>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
@@ -3318,8 +3383,12 @@
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="8"/>
+      <c r="R6" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="T6" s="8"/>
       <c r="U6" s="8"/>
       <c r="V6" s="8"/>
@@ -3380,10 +3449,18 @@
         <v>109</v>
       </c>
       <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
+      <c r="R7" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="S7" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8"/>
@@ -3396,7 +3473,7 @@
       <c r="AE7" s="7"/>
       <c r="AF7" s="7"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -3417,18 +3494,40 @@
         <v>26</v>
       </c>
       <c r="H8" s="7"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
+      <c r="I8" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
+      <c r="R8" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>115</v>
+      </c>
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
@@ -3928,4 +4027,982 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1508A462-E7B4-4644-A273-210A4926AFD4}">
+  <dimension ref="A1:AF21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" style="1" customWidth="1"/>
+    <col min="20" max="21" width="19.140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="16.5703125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="16.7109375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="17.140625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="16.140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="21.140625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="30.85546875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="17" style="1" customWidth="1"/>
+    <col min="31" max="31" width="15.7109375" style="1" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+    </row>
+    <row r="2" spans="1:32" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+    </row>
+    <row r="3" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="O3" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="P3" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="S3" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="T3" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="U3" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="V3" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="W3" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="X3" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="19"/>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
+    </row>
+    <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+    </row>
+    <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+    </row>
+    <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="W7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="X7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="7"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="7"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="8"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="5"/>
+      <c r="AF18" s="7"/>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
+      <c r="AF19" s="7"/>
+    </row>
+    <row r="20" spans="1:32" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="7"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="7"/>
+      <c r="AF20" s="7"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="8"/>
+      <c r="AE21" s="7"/>
+      <c r="AF21" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AF1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{9360D4F5-6234-46FF-96C1-6B5BAE55F411}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{52B5FE61-9D1B-4DE4-9333-F478D65E434A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Checkout feature is added
</commit_message>
<xml_diff>
--- a/src/test/test_data/ipon.xlsx
+++ b/src/test/test_data/ipon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\QAprojekti\Automation_projekti\iponhu\src\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23663BE-FA2C-4087-B615-A776D132DF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549D9F04-D79E-4683-98C8-5B7EE622B8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47DA7BBC-4371-411F-99D1-AFF8C5BF69E2}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="136">
   <si>
     <t>tc_id</t>
   </si>
@@ -384,6 +384,12 @@
     <t>rgba(239, 68, 68, 1)</t>
   </si>
   <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
     <t>zipcodeMessage</t>
   </si>
   <si>
@@ -391,6 +397,45 @@
   </si>
   <si>
     <t>streetMessage</t>
+  </si>
+  <si>
+    <t>This value is not a valid zip code.</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>3300</t>
+  </si>
+  <si>
+    <t>Hajduk Veljkova</t>
+  </si>
+  <si>
+    <t>otherData</t>
+  </si>
+  <si>
+    <t>201234567</t>
+  </si>
+  <si>
+    <t>NIKOLA STJEPANOVIC</t>
+  </si>
+  <si>
+    <t>3300 Eger, Hajduk Veljkova</t>
   </si>
 </sst>
 </file>
@@ -899,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D05107-472F-4DD1-88F8-DE97CAF36E00}">
   <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,11 +969,12 @@
     <col min="18" max="18" width="21.5703125" style="1" customWidth="1"/>
     <col min="19" max="19" width="11.5703125" style="1" customWidth="1"/>
     <col min="20" max="20" width="14.28515625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="19.42578125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="19.5703125" style="1" customWidth="1"/>
-    <col min="24" max="25" width="19.140625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5703125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="5.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="8" style="1" customWidth="1"/>
+    <col min="24" max="24" width="13" style="1" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="23.28515625" style="1" customWidth="1"/>
     <col min="27" max="28" width="16.7109375" style="1" customWidth="1"/>
     <col min="29" max="29" width="17.140625" style="1" customWidth="1"/>
     <col min="30" max="30" width="16.42578125" style="1" customWidth="1"/>
@@ -1045,12 +1091,24 @@
       <c r="T3" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
+      <c r="U3" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>132</v>
+      </c>
       <c r="AA3" s="6"/>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
@@ -1117,12 +1175,22 @@
       <c r="T4" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
+      <c r="U4" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
+      <c r="X4" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z4" s="7" t="s">
+        <v>135</v>
+      </c>
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
       <c r="AC4" s="7"/>
@@ -4033,8 +4101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1508A462-E7B4-4644-A273-210A4926AFD4}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4061,7 +4129,7 @@
     <col min="20" max="21" width="19.140625" style="1" customWidth="1"/>
     <col min="22" max="22" width="16.5703125" style="1" customWidth="1"/>
     <col min="23" max="24" width="16.7109375" style="1" customWidth="1"/>
-    <col min="25" max="25" width="17.140625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="12.42578125" style="1" customWidth="1"/>
     <col min="26" max="26" width="16.42578125" style="1" customWidth="1"/>
     <col min="27" max="27" width="16.140625" style="1" customWidth="1"/>
     <col min="28" max="28" width="21.140625" style="1" customWidth="1"/>
@@ -4174,18 +4242,26 @@
         <v>116</v>
       </c>
       <c r="V3" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="W3" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="X3" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y3" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z3" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA3" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="W3" s="19" t="s">
+      <c r="AB3" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="X3" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y3" s="19"/>
-      <c r="Z3" s="19"/>
-      <c r="AA3" s="19"/>
-      <c r="AB3" s="19"/>
       <c r="AC3" s="19"/>
       <c r="AD3" s="19"/>
       <c r="AE3" s="19"/>
@@ -4247,11 +4323,21 @@
       </c>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
+      <c r="V4" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="W4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="X4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z4" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
       <c r="AC4" s="7"/>
@@ -4313,7 +4399,6 @@
       </c>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
       <c r="W5" s="7"/>
       <c r="X5" s="7"/>
       <c r="Y5" s="7"/>
@@ -4507,7 +4592,6 @@
         <v>115</v>
       </c>
       <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
       <c r="W8" s="7"/>
       <c r="X8" s="7"/>
       <c r="Y8" s="7"/>

</xml_diff>